<commit_message>
AlterarSenha - Ver funcionario
</commit_message>
<xml_diff>
--- a/DOCS/Planejamento PBD.xlsx
+++ b/DOCS/Planejamento PBD.xlsx
@@ -370,6 +370,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -377,30 +378,29 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,15 +731,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
@@ -752,99 +752,99 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="20">
         <v>43374</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="20">
         <v>43466</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10" s="21">
         <v>0.12</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -870,14 +870,14 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -903,19 +903,19 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B15" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="14">
         <v>43389</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="22">
         <v>43393</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="15">
         <v>5</v>
       </c>
       <c r="F15" s="8" t="s">
@@ -926,13 +926,13 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
+      <c r="A16" s="16"/>
       <c r="B16" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="15"/>
       <c r="F16" s="8" t="s">
         <v>24</v>
       </c>
@@ -941,13 +941,13 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
+      <c r="A17" s="16"/>
       <c r="B17" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="15"/>
       <c r="F17" s="8" t="s">
         <v>24</v>
       </c>
@@ -979,19 +979,19 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B19" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="22">
         <v>43402</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="22">
         <v>43378</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="15">
         <v>8</v>
       </c>
       <c r="F19" t="s">
@@ -1002,13 +1002,13 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
+      <c r="A20" s="16"/>
       <c r="B20" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="14"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="15"/>
       <c r="F20" t="s">
         <v>24</v>
       </c>
@@ -1017,13 +1017,13 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
+      <c r="A21" s="16"/>
       <c r="B21" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="14"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="15"/>
       <c r="F21" t="s">
         <v>35</v>
       </c>
@@ -1032,19 +1032,19 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="16" t="s">
         <v>36</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="14">
         <v>43410</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="14">
         <v>43414</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="15">
         <v>4</v>
       </c>
       <c r="F22" s="6" t="s">
@@ -1055,13 +1055,13 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="15"/>
       <c r="F23" t="s">
         <v>32</v>
       </c>
@@ -1070,13 +1070,13 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="15"/>
       <c r="F24" t="s">
         <v>24</v>
       </c>
@@ -1108,19 +1108,19 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="16" t="s">
         <v>44</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C26" s="14">
         <v>43421</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="14">
         <v>43426</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="15">
         <v>5</v>
       </c>
       <c r="F26" s="6" t="s">
@@ -1131,13 +1131,13 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="15"/>
       <c r="F27" t="s">
         <v>48</v>
       </c>
@@ -1146,13 +1146,13 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
+      <c r="A28" s="16"/>
       <c r="B28" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="15"/>
       <c r="F28" t="s">
         <v>50</v>
       </c>
@@ -1161,51 +1161,51 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="16" t="s">
         <v>51</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="13">
+      <c r="C29" s="14">
         <v>43427</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D29" s="14">
         <v>43431</v>
       </c>
-      <c r="E29" s="14">
+      <c r="E29" s="15">
         <v>2</v>
       </c>
       <c r="F29" t="s">
         <v>53</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="15"/>
       <c r="F30" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="15"/>
       <c r="F31" t="s">
         <v>57</v>
       </c>
@@ -1233,40 +1233,40 @@
         <v>43</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="H32" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="I32" s="23" t="s">
+      <c r="I32" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="23" t="s">
         <v>61</v>
       </c>
       <c r="B34" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13">
+      <c r="C34" s="14">
         <v>43444</v>
       </c>
-      <c r="D34" s="13">
+      <c r="D34" s="14">
         <v>43452</v>
       </c>
-      <c r="E34" s="14">
+      <c r="E34" s="15">
         <v>8</v>
       </c>
       <c r="F34" t="s">
@@ -1277,13 +1277,13 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
+      <c r="A35" s="23"/>
       <c r="B35" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="15"/>
       <c r="F35" t="s">
         <v>38</v>
       </c>
@@ -1292,13 +1292,13 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
+      <c r="A36" s="23"/>
       <c r="B36" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="15"/>
       <c r="F36" t="s">
         <v>38</v>
       </c>
@@ -1330,19 +1330,19 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="15" t="s">
         <v>68</v>
       </c>
       <c r="B38" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="13">
+      <c r="C38" s="14">
         <v>43460</v>
       </c>
-      <c r="D38" s="13">
+      <c r="D38" s="14">
         <v>43493</v>
       </c>
-      <c r="E38" s="14">
+      <c r="E38" s="15">
         <v>28</v>
       </c>
       <c r="F38" t="s">
@@ -1353,13 +1353,13 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
+      <c r="A39" s="15"/>
       <c r="B39" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="15"/>
       <c r="F39" t="s">
         <v>72</v>
       </c>
@@ -1368,13 +1368,13 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
+      <c r="A40" s="15"/>
       <c r="B40" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="15"/>
       <c r="F40" t="s">
         <v>74</v>
       </c>
@@ -1383,13 +1383,13 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
+      <c r="A41" s="15"/>
       <c r="B41" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="15"/>
       <c r="F41" t="s">
         <v>76</v>
       </c>
@@ -1398,13 +1398,13 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
+      <c r="A42" s="15"/>
       <c r="B42" t="s">
         <v>77</v>
       </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="15"/>
       <c r="F42" t="s">
         <v>78</v>
       </c>
@@ -1413,13 +1413,13 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
+      <c r="A43" s="15"/>
       <c r="B43" t="s">
         <v>79</v>
       </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="15"/>
       <c r="F43" t="s">
         <v>80</v>
       </c>
@@ -1428,13 +1428,13 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
+      <c r="A44" s="15"/>
       <c r="B44" t="s">
         <v>81</v>
       </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="15"/>
       <c r="F44" t="s">
         <v>82</v>
       </c>
@@ -1443,13 +1443,13 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
+      <c r="A45" s="15"/>
       <c r="B45" t="s">
         <v>83</v>
       </c>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="14"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="15"/>
       <c r="F45" t="s">
         <v>84</v>
       </c>
@@ -1459,37 +1459,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
     <mergeCell ref="C38:C45"/>
     <mergeCell ref="D38:D45"/>
     <mergeCell ref="E38:E45"/>
@@ -1499,6 +1468,37 @@
     <mergeCell ref="C34:C36"/>
     <mergeCell ref="D34:D36"/>
     <mergeCell ref="E34:E36"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A26:A28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finalizado (mais ou menos)
</commit_message>
<xml_diff>
--- a/DOCS/Planejamento PBD.xlsx
+++ b/DOCS/Planejamento PBD.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
   <si>
     <t>Plano de Projeto da Disciplina de PBD - Turma 2018.2</t>
   </si>
@@ -188,9 +188,6 @@
   </si>
   <si>
     <t>2h</t>
-  </si>
-  <si>
-    <t>Atrasado</t>
   </si>
   <si>
     <t>criar senha</t>
@@ -378,28 +375,28 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -718,7 +715,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,15 +728,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
@@ -752,55 +749,55 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -839,12 +836,12 @@
       <c r="F10" s="21"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -870,14 +867,14 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -903,7 +900,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="18" t="s">
         <v>22</v>
       </c>
       <c r="B15" t="s">
@@ -912,7 +909,7 @@
       <c r="C15" s="14">
         <v>43389</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="19">
         <v>43393</v>
       </c>
       <c r="E15" s="15">
@@ -926,12 +923,12 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
+      <c r="A16" s="18"/>
       <c r="B16" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="14"/>
-      <c r="D16" s="22"/>
+      <c r="D16" s="19"/>
       <c r="E16" s="15"/>
       <c r="F16" s="8" t="s">
         <v>24</v>
@@ -941,12 +938,12 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
+      <c r="A17" s="18"/>
       <c r="B17" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="14"/>
-      <c r="D17" s="22"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="15"/>
       <c r="F17" s="8" t="s">
         <v>24</v>
@@ -979,16 +976,16 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="18" t="s">
         <v>30</v>
       </c>
       <c r="B19" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="22">
+      <c r="C19" s="19">
         <v>43402</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19" s="19">
         <v>43378</v>
       </c>
       <c r="E19" s="15">
@@ -1002,12 +999,12 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
+      <c r="A20" s="18"/>
       <c r="B20" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
       <c r="E20" s="15"/>
       <c r="F20" t="s">
         <v>24</v>
@@ -1017,12 +1014,12 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
+      <c r="A21" s="18"/>
       <c r="B21" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
       <c r="E21" s="15"/>
       <c r="F21" t="s">
         <v>35</v>
@@ -1032,7 +1029,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="18" t="s">
         <v>36</v>
       </c>
       <c r="B22" s="6" t="s">
@@ -1055,7 +1052,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
+      <c r="A23" s="18"/>
       <c r="B23" s="6" t="s">
         <v>39</v>
       </c>
@@ -1070,7 +1067,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="6" t="s">
         <v>40</v>
       </c>
@@ -1108,7 +1105,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="18" t="s">
         <v>44</v>
       </c>
       <c r="B26" s="6" t="s">
@@ -1131,7 +1128,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="6" t="s">
         <v>47</v>
       </c>
@@ -1146,7 +1143,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="6" t="s">
         <v>49</v>
       </c>
@@ -1161,7 +1158,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="18" t="s">
         <v>51</v>
       </c>
       <c r="B29" s="6" t="s">
@@ -1184,9 +1181,9 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C30" s="14"/>
       <c r="D30" s="14"/>
@@ -1199,26 +1196,26 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C31" s="14"/>
       <c r="D31" s="14"/>
       <c r="E31" s="15"/>
       <c r="F31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>59</v>
       </c>
       <c r="C32" s="7">
         <v>43432</v>
@@ -1236,29 +1233,29 @@
         <v>21</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I32" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="23" t="s">
+      <c r="B34" t="s">
         <v>61</v>
-      </c>
-      <c r="B34" t="s">
-        <v>62</v>
       </c>
       <c r="C34" s="14">
         <v>43444</v>
@@ -1273,13 +1270,13 @@
         <v>46</v>
       </c>
       <c r="G34" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="17"/>
+      <c r="B35" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
-      <c r="B35" t="s">
-        <v>64</v>
       </c>
       <c r="C35" s="14"/>
       <c r="D35" s="14"/>
@@ -1288,13 +1285,13 @@
         <v>38</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
+      <c r="A36" s="17"/>
       <c r="B36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C36" s="14"/>
       <c r="D36" s="14"/>
@@ -1303,15 +1300,15 @@
         <v>38</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>67</v>
       </c>
       <c r="C37" s="9">
         <v>43453</v>
@@ -1326,15 +1323,15 @@
         <v>53</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" t="s">
         <v>68</v>
-      </c>
-      <c r="B38" t="s">
-        <v>69</v>
       </c>
       <c r="C38" s="14">
         <v>43460</v>
@@ -1346,119 +1343,150 @@
         <v>28</v>
       </c>
       <c r="F38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="B39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C39" s="14"/>
       <c r="D39" s="14"/>
       <c r="E39" s="15"/>
       <c r="F39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
       <c r="B40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C40" s="14"/>
       <c r="D40" s="14"/>
       <c r="E40" s="15"/>
       <c r="F40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C41" s="14"/>
       <c r="D41" s="14"/>
       <c r="E41" s="15"/>
       <c r="F41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="15"/>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C42" s="14"/>
       <c r="D42" s="14"/>
       <c r="E42" s="15"/>
       <c r="F42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
       <c r="B43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C43" s="14"/>
       <c r="D43" s="14"/>
       <c r="E43" s="15"/>
       <c r="F43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>
       <c r="B44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C44" s="14"/>
       <c r="D44" s="14"/>
       <c r="E44" s="15"/>
       <c r="F44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C45" s="14"/>
       <c r="D45" s="14"/>
       <c r="E45" s="15"/>
       <c r="F45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
     <mergeCell ref="C38:C45"/>
     <mergeCell ref="D38:D45"/>
     <mergeCell ref="E38:E45"/>
@@ -1468,37 +1496,6 @@
     <mergeCell ref="C34:C36"/>
     <mergeCell ref="D34:D36"/>
     <mergeCell ref="E34:E36"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A26:A28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>